<commit_message>
following protocol for selecting variables
</commit_message>
<xml_diff>
--- a/Documents/PredictorScreeningTable.xlsx
+++ b/Documents/PredictorScreeningTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarahhart/Library/CloudStorage/GoogleDrive-sarahjanehart13@gmail.com/My Drive/RESEARCH/Analyses/AspenHabitat/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B91E3E6-D500-A84C-8EA2-4DB66D590ED3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C306181-1302-434F-9D42-845F9E6B6253}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-6020" windowWidth="21560" windowHeight="21100" xr2:uid="{EC5E61FB-4842-014B-8360-6D6CF19886B2}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{EC5E61FB-4842-014B-8360-6D6CF19886B2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="119">
   <si>
     <t>Variable</t>
   </si>
@@ -383,9 +383,6 @@
   </si>
   <si>
     <t>Identified as important predictor by Rehfeldt et al. (2009) and (2015).</t>
-  </si>
-  <si>
-    <t>Group preference order</t>
   </si>
   <si>
     <t>Temperature-precip</t>
@@ -829,24 +826,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1C5EC75-8A6B-F240-9538-D6820B489B90}">
-  <dimension ref="A1:H36"/>
+  <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B15" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="0" style="9" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="9" customWidth="1"/>
     <col min="2" max="2" width="10.83203125" style="9"/>
     <col min="3" max="4" width="24.6640625" style="10" customWidth="1"/>
     <col min="5" max="6" width="10.83203125" style="10"/>
-    <col min="7" max="7" width="11.5" style="10" customWidth="1"/>
-    <col min="8" max="8" width="35.5" style="10" customWidth="1"/>
-    <col min="9" max="16384" width="10.83203125" style="9"/>
+    <col min="7" max="7" width="35.5" style="10" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="8" customFormat="1" ht="51">
+    <row r="1" spans="1:7" s="8" customFormat="1" ht="34">
       <c r="A1" s="13" t="s">
         <v>102</v>
       </c>
@@ -866,15 +862,12 @@
         <v>106</v>
       </c>
       <c r="G1" s="14" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="51">
+      <c r="A2" s="15" t="s">
         <v>115</v>
-      </c>
-      <c r="H1" s="14" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="51">
-      <c r="A2" s="15" t="s">
-        <v>116</v>
       </c>
       <c r="B2" s="13" t="s">
         <v>3</v>
@@ -891,14 +884,11 @@
       <c r="F2" s="18">
         <v>1</v>
       </c>
-      <c r="G2" s="16">
-        <v>1</v>
-      </c>
-      <c r="H2" s="16" t="s">
+      <c r="G2" s="16" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="34">
+    <row r="3" spans="1:7" ht="34">
       <c r="A3" s="15" t="s">
         <v>105</v>
       </c>
@@ -915,17 +905,13 @@
       <c r="F3" s="18">
         <v>28</v>
       </c>
-      <c r="G3" s="16">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="H3" s="16" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="45" customHeight="1">
+      <c r="G3" s="16" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="45" customHeight="1">
       <c r="A4" s="15" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B4" s="15" t="s">
         <v>10</v>
@@ -940,17 +926,13 @@
       <c r="F4" s="18">
         <v>17</v>
       </c>
-      <c r="G4" s="16">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="H4" s="16" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="34">
+      <c r="G4" s="16" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="34">
       <c r="A5" s="15" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B5" s="15" t="s">
         <v>11</v>
@@ -965,15 +947,11 @@
       <c r="F5" s="18">
         <v>11</v>
       </c>
-      <c r="G5" s="16">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="H5" s="16" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="17">
+      <c r="G5" s="16" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="17">
       <c r="A6" s="15" t="s">
         <v>105</v>
       </c>
@@ -990,15 +968,11 @@
       <c r="F6" s="18">
         <v>15</v>
       </c>
-      <c r="G6" s="16">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="H6" s="16" t="s">
+      <c r="G6" s="16" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="34">
+    <row r="7" spans="1:7" ht="34">
       <c r="A7" s="15" t="s">
         <v>105</v>
       </c>
@@ -1015,15 +989,11 @@
       <c r="F7" s="18">
         <v>12</v>
       </c>
-      <c r="G7" s="16">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="H7" s="16" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="34">
+      <c r="G7" s="16" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="34">
       <c r="A8" s="15" t="s">
         <v>105</v>
       </c>
@@ -1040,15 +1010,11 @@
       <c r="F8" s="18">
         <v>16</v>
       </c>
-      <c r="G8" s="16">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="H8" s="16" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="34">
+      <c r="G8" s="16" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="34">
       <c r="A9" s="15" t="s">
         <v>105</v>
       </c>
@@ -1065,15 +1031,11 @@
       <c r="F9" s="18">
         <v>21</v>
       </c>
-      <c r="G9" s="16">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="H9" s="16" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="68">
+      <c r="G9" s="16" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="68">
       <c r="A10" s="15" t="s">
         <v>105</v>
       </c>
@@ -1092,14 +1054,11 @@
       <c r="F10" s="18">
         <v>3</v>
       </c>
-      <c r="G10" s="16">
-        <v>1</v>
-      </c>
-      <c r="H10" s="16" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="34">
+      <c r="G10" s="16" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="34">
       <c r="A11" s="15" t="s">
         <v>105</v>
       </c>
@@ -1116,15 +1075,11 @@
       <c r="F11" s="18">
         <v>33</v>
       </c>
-      <c r="G11" s="16">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="H11" s="16" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="34">
+      <c r="G11" s="16" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="34">
       <c r="A12" s="15" t="s">
         <v>103</v>
       </c>
@@ -1141,17 +1096,13 @@
       <c r="F12" s="18">
         <v>26</v>
       </c>
-      <c r="G12" s="16">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="H12" s="16" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="34">
+      <c r="G12" s="16" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="34">
       <c r="A13" s="15" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B13" s="15" t="s">
         <v>19</v>
@@ -1166,15 +1117,11 @@
       <c r="F13" s="18">
         <v>18</v>
       </c>
-      <c r="G13" s="16">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="H13" s="16" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="34">
+      <c r="G13" s="16" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="34">
       <c r="A14" s="15" t="s">
         <v>103</v>
       </c>
@@ -1191,15 +1138,11 @@
       <c r="F14" s="18">
         <v>30</v>
       </c>
-      <c r="G14" s="16">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="H14" s="16" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="34">
+      <c r="G14" s="16" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="34">
       <c r="A15" s="15" t="s">
         <v>105</v>
       </c>
@@ -1216,15 +1159,11 @@
       <c r="F15" s="18">
         <v>31</v>
       </c>
-      <c r="G15" s="16">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="H15" s="16" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="33" customHeight="1">
+      <c r="G15" s="16" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="33" customHeight="1">
       <c r="A16" s="15" t="s">
         <v>104</v>
       </c>
@@ -1243,16 +1182,13 @@
       <c r="F16" s="18">
         <v>8</v>
       </c>
-      <c r="G16" s="16">
-        <v>1</v>
-      </c>
-      <c r="H16" s="16" t="s">
+      <c r="G16" s="16" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="51">
+    <row r="17" spans="1:7" ht="51">
       <c r="A17" s="15" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B17" s="13" t="s">
         <v>4</v>
@@ -1269,14 +1205,11 @@
       <c r="F17" s="18">
         <v>5</v>
       </c>
-      <c r="G17" s="16">
-        <v>2</v>
-      </c>
-      <c r="H17" s="16" t="s">
+      <c r="G17" s="16" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="51">
+    <row r="18" spans="1:7" ht="51">
       <c r="A18" s="15" t="s">
         <v>104</v>
       </c>
@@ -1295,14 +1228,11 @@
       <c r="F18" s="18">
         <v>6</v>
       </c>
-      <c r="G18" s="16">
-        <v>1</v>
-      </c>
-      <c r="H18" s="16" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="34">
+      <c r="G18" s="16" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="34">
       <c r="A19" s="15" t="s">
         <v>103</v>
       </c>
@@ -1319,15 +1249,11 @@
       <c r="F19" s="18">
         <v>22</v>
       </c>
-      <c r="G19" s="16">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="H19" s="16" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="34">
+      <c r="G19" s="16" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="34">
       <c r="A20" s="15" t="s">
         <v>103</v>
       </c>
@@ -1344,15 +1270,11 @@
       <c r="F20" s="18">
         <v>20</v>
       </c>
-      <c r="G20" s="16">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="H20" s="16" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="51">
+      <c r="G20" s="16" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="51">
       <c r="A21" s="15" t="s">
         <v>103</v>
       </c>
@@ -1371,14 +1293,11 @@
       <c r="F21" s="18">
         <v>9</v>
       </c>
-      <c r="G21" s="16">
-        <v>2</v>
-      </c>
-      <c r="H21" s="16" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="34">
+      <c r="G21" s="16" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="34">
       <c r="A22" s="15" t="s">
         <v>105</v>
       </c>
@@ -1395,15 +1314,11 @@
       <c r="F22" s="18">
         <v>29</v>
       </c>
-      <c r="G22" s="16">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="H22" s="16" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="68">
+      <c r="G22" s="16" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="68">
       <c r="A23" s="15" t="s">
         <v>104</v>
       </c>
@@ -1420,15 +1335,11 @@
       <c r="F23" s="18">
         <v>13</v>
       </c>
-      <c r="G23" s="16">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="H23" s="16" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="34">
+      <c r="G23" s="16" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="34">
       <c r="A24" s="15" t="s">
         <v>104</v>
       </c>
@@ -1445,15 +1356,11 @@
       <c r="F24" s="18">
         <v>14</v>
       </c>
-      <c r="G24" s="16">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="H24" s="16" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="34">
+      <c r="G24" s="16" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="34">
       <c r="A25" s="15" t="s">
         <v>104</v>
       </c>
@@ -1470,15 +1377,11 @@
       <c r="F25" s="18">
         <v>32</v>
       </c>
-      <c r="G25" s="16">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="H25" s="16" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="34">
+      <c r="G25" s="16" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="34">
       <c r="A26" s="15" t="s">
         <v>104</v>
       </c>
@@ -1495,15 +1398,11 @@
       <c r="F26" s="18">
         <v>19</v>
       </c>
-      <c r="G26" s="16">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="H26" s="16" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="51">
+      <c r="G26" s="16" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="51">
       <c r="A27" s="15" t="s">
         <v>104</v>
       </c>
@@ -1522,14 +1421,11 @@
       <c r="F27" s="18">
         <v>7</v>
       </c>
-      <c r="G27" s="16">
-        <v>1</v>
-      </c>
-      <c r="H27" s="16" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="51">
+      <c r="G27" s="16" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="51">
       <c r="A28" s="15" t="s">
         <v>104</v>
       </c>
@@ -1548,16 +1444,13 @@
       <c r="F28" s="18">
         <v>2</v>
       </c>
-      <c r="G28" s="16">
-        <v>1</v>
-      </c>
-      <c r="H28" s="16" t="s">
+      <c r="G28" s="16" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="34">
+    <row r="29" spans="1:7" ht="34">
       <c r="A29" s="15" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B29" s="15" t="s">
         <v>35</v>
@@ -1572,15 +1465,11 @@
       <c r="F29" s="18">
         <v>34</v>
       </c>
-      <c r="G29" s="16">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="H29" s="16" t="s">
+      <c r="G29" s="16" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="34">
+    <row r="30" spans="1:7" ht="34">
       <c r="A30" s="15" t="s">
         <v>103</v>
       </c>
@@ -1597,15 +1486,11 @@
       <c r="F30" s="18">
         <v>27</v>
       </c>
-      <c r="G30" s="16">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="H30" s="16" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" ht="34">
+      <c r="G30" s="16" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="34">
       <c r="A31" s="15" t="s">
         <v>103</v>
       </c>
@@ -1622,15 +1507,11 @@
       <c r="F31" s="18">
         <v>24</v>
       </c>
-      <c r="G31" s="16">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="H31" s="16" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" ht="34">
+      <c r="G31" s="16" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="34">
       <c r="A32" s="15" t="s">
         <v>103</v>
       </c>
@@ -1647,15 +1528,11 @@
       <c r="F32" s="18">
         <v>25</v>
       </c>
-      <c r="G32" s="16">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="H32" s="16" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" ht="34">
+      <c r="G32" s="16" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="34">
       <c r="A33" s="15" t="s">
         <v>103</v>
       </c>
@@ -1672,15 +1549,11 @@
       <c r="F33" s="18">
         <v>23</v>
       </c>
-      <c r="G33" s="16">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="H33" s="16" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" ht="68">
+      <c r="G33" s="16" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="68">
       <c r="A34" s="15" t="s">
         <v>105</v>
       </c>
@@ -1699,14 +1572,11 @@
       <c r="F34" s="18">
         <v>10</v>
       </c>
-      <c r="G34" s="16">
-        <v>1</v>
-      </c>
-      <c r="H34" s="16" t="s">
+      <c r="G34" s="16" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="68">
+    <row r="35" spans="1:7" ht="68">
       <c r="A35" s="15" t="s">
         <v>103</v>
       </c>
@@ -1725,23 +1595,19 @@
       <c r="F35" s="18">
         <v>4</v>
       </c>
-      <c r="G35" s="16">
-        <v>1</v>
-      </c>
-      <c r="H35" s="16" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8">
+      <c r="G35" s="16" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
       <c r="C36" s="9"/>
       <c r="D36" s="9"/>
       <c r="E36" s="9"/>
       <c r="F36" s="9"/>
       <c r="G36" s="9"/>
-      <c r="H36" s="9"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H35">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G35">
     <sortCondition ref="B2:B35"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
draft for co-author review
</commit_message>
<xml_diff>
--- a/Documents/PredictorScreeningTable.xlsx
+++ b/Documents/PredictorScreeningTable.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarahhart/Library/CloudStorage/GoogleDrive-sarahjanehart13@gmail.com/My Drive/JOB/RESEARCH/Analyses/AspenHabitat/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C521862E-6EB1-0D40-9C91-8908E3007958}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD351892-038C-1643-8D4C-34B112D33FC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23040" yWindow="700" windowWidth="30240" windowHeight="19640" activeTab="1" xr2:uid="{EC5E61FB-4842-014B-8360-6D6CF19886B2}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{EC5E61FB-4842-014B-8360-6D6CF19886B2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -379,9 +379,6 @@
     <t>Drop out loss</t>
   </si>
   <si>
-    <t xml:space="preserve"> (Rehfeldt et al. 2009).</t>
-  </si>
-  <si>
     <t>growing season precipitation  degree day ratio: (GSP*DD5/1000)</t>
   </si>
   <si>
@@ -389,6 +386,9 @@
   </si>
   <si>
     <t>SWC</t>
+  </si>
+  <si>
+    <t>Plant productivity is higher in areas with warmer temperatures and greater preciptiation during the growing season  (Rehfeldt et al. 2009).</t>
   </si>
 </sst>
 </file>
@@ -1455,7 +1455,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1509,15 +1509,15 @@
         <v>79</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="34">
+    <row r="5" spans="1:3" ht="51">
       <c r="A5" s="6" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="51">
@@ -1566,7 +1566,7 @@
     </row>
     <row r="10" spans="1:3" ht="34">
       <c r="A10" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>99</v>
@@ -1577,7 +1577,7 @@
     </row>
     <row r="11" spans="1:3" ht="34">
       <c r="A11" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>101</v>

</xml_diff>